<commit_message>
cap nhat thu lai thu goc
</commit_message>
<xml_diff>
--- a/insoden/thugoclai.xlsx
+++ b/insoden/thugoclai.xlsx
@@ -9,11 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="120" yWindow="15" windowWidth="15195" windowHeight="8190" tabRatio="852"/>
+    <workbookView xWindow="120" yWindow="15" windowWidth="15195" windowHeight="8190" tabRatio="852" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="9" r:id="rId1"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId2"/>
+    <sheet name="GDN" sheetId="9" r:id="rId1"/>
+    <sheet name="ChiTiet" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
 </workbook>
@@ -691,8 +691,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H21" sqref="H21"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1490,7 +1490,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>

</xml_diff>

<commit_message>
cap nhat loi hien cif va ten thu goc lai
</commit_message>
<xml_diff>
--- a/insoden/thugoclai.xlsx
+++ b/insoden/thugoclai.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="17030"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="17127"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="120" yWindow="15" windowWidth="15195" windowHeight="8190" tabRatio="852" activeTab="1"/>
+    <workbookView xWindow="120" yWindow="15" windowWidth="15195" windowHeight="8190" tabRatio="852"/>
   </bookViews>
   <sheets>
     <sheet name="GDN" sheetId="9" r:id="rId1"/>
@@ -691,8 +691,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5:H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -703,7 +703,7 @@
     <col min="5" max="5" width="11" customWidth="1"/>
     <col min="6" max="6" width="18.875" customWidth="1"/>
     <col min="7" max="7" width="21.75" customWidth="1"/>
-    <col min="8" max="8" width="10.125" customWidth="1"/>
+    <col min="8" max="8" width="9.5" customWidth="1"/>
     <col min="257" max="257" width="5.125" customWidth="1"/>
     <col min="258" max="258" width="22.25" customWidth="1"/>
     <col min="259" max="259" width="14.375" customWidth="1"/>
@@ -1490,7 +1490,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>

</xml_diff>